<commit_message>
Add escrow and trading UI images
</commit_message>
<xml_diff>
--- a/FSMP calculation.xlsx
+++ b/FSMP calculation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHESTER\Dropbox\FSMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHESTER\Git\fsmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="105">
   <si>
     <t>Average Peers Quantity</t>
   </si>
@@ -336,6 +336,12 @@
   </si>
   <si>
     <t>$2.40</t>
+  </si>
+  <si>
+    <t>Open Date</t>
+  </si>
+  <si>
+    <t>Close Date</t>
   </si>
 </sst>
 </file>
@@ -909,7 +915,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1119,10 +1125,10 @@
         <v>78</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="G11" s="35" t="s">
         <v>66</v>

</xml_diff>